<commit_message>
Start recog from target | wait for fin_in_start_point
</commit_message>
<xml_diff>
--- a/development/Code_Output_Explanation.xlsx
+++ b/development/Code_Output_Explanation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\university\mudrick_lab\codes\subliminal_priming\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\university\mudrick_lab\subliminal_priming_w_motion_capture\development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5DF02D8-6342-42BD-B89F-978B3F9D55EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F932284F-245D-497F-A7C5-43568C0E70F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="615" yWindow="615" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="79">
   <si>
     <t>prime</t>
   </si>
@@ -219,6 +219,60 @@
   </si>
   <si>
     <t>target_timecourse</t>
+  </si>
+  <si>
+    <t>fix_duration</t>
+  </si>
+  <si>
+    <t>mask1_duration</t>
+  </si>
+  <si>
+    <t>mask2_duration</t>
+  </si>
+  <si>
+    <t>prime_duration</t>
+  </si>
+  <si>
+    <t>mask3_duration</t>
+  </si>
+  <si>
+    <t>target_duration</t>
+  </si>
+  <si>
+    <t>timestamp when fixation was displayed</t>
+  </si>
+  <si>
+    <t>timestamp when mask1 was displayed</t>
+  </si>
+  <si>
+    <t>categor_time</t>
+  </si>
+  <si>
+    <t>recog_time</t>
+  </si>
+  <si>
+    <t>pas_time</t>
+  </si>
+  <si>
+    <t>timestamp when mask2 was displayed</t>
+  </si>
+  <si>
+    <t>timestamp when prime was displayed</t>
+  </si>
+  <si>
+    <t>timestamp when mask3 was displayed</t>
+  </si>
+  <si>
+    <t>timestamp when target was displayed</t>
+  </si>
+  <si>
+    <t>timestamp when categorization task was displayed</t>
+  </si>
+  <si>
+    <t>timestamp when recognition task was displayed</t>
+  </si>
+  <si>
+    <t>timestamp when PAS task was displayed</t>
   </si>
 </sst>
 </file>
@@ -540,18 +594,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AK2"/>
+  <dimension ref="A1:AT2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z3" sqref="Z3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.25" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="37" max="37" width="20.5" customWidth="1"/>
+    <col min="46" max="46" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -586,85 +640,112 @@
         <v>55</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="X1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:46" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>29</v>
@@ -711,61 +792,88 @@
         <v>27</v>
       </c>
       <c r="R2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="AF2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="AG2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AP2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AH2" s="1"/>
-      <c r="AI2" s="1" t="s">
+      <c r="AQ2" s="1"/>
+      <c r="AR2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AJ2" s="1" t="s">
+      <c r="AS2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AK2" s="1" t="s">
+      <c r="AT2" s="1" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Erase first row instead od iteration on trials
</commit_message>
<xml_diff>
--- a/development/Code_Output_Explanation.xlsx
+++ b/development/Code_Output_Explanation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\university\mudrick_lab\subliminal_priming_w_motion_capture\development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F932284F-245D-497F-A7C5-43568C0E70F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A049C9-9F65-4B49-AA1D-CDBDF9542C64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="81">
   <si>
     <t>prime</t>
   </si>
@@ -273,6 +273,12 @@
   </si>
   <si>
     <t>timestamp when PAS task was displayed</t>
+  </si>
+  <si>
+    <t>sub_num</t>
+  </si>
+  <si>
+    <t>subject number</t>
   </si>
 </sst>
 </file>
@@ -594,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AT2"/>
+  <dimension ref="A1:AU2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z3" sqref="Z3"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AU3" sqref="AU3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.25" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -605,7 +611,7 @@
     <col min="46" max="46" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -744,8 +750,11 @@
       <c r="AT1" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="AU1" s="1" t="s">
+        <v>79</v>
+      </c>
     </row>
-    <row r="2" spans="1:46" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:47" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>29</v>
@@ -875,6 +884,9 @@
       </c>
       <c r="AT2" s="1" t="s">
         <v>52</v>
+      </c>
+      <c r="AU2" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Debug | Fix save data to file | Split traj to xyz in trials table
Debug last commits.
Fixed events timings.
Added blue touch dots.
</commit_message>
<xml_diff>
--- a/development/Code_Output_Explanation.xlsx
+++ b/development/Code_Output_Explanation.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\university\mudrick_lab\subliminal_priming_w_motion_capture\development\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\khen_heller\subliminal_priming_w_motion_capture-main\development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A049C9-9F65-4B49-AA1D-CDBDF9542C64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="89">
   <si>
     <t>prime</t>
   </si>
@@ -135,12 +134,6 @@
     <t>target_ans_nat</t>
   </si>
   <si>
-    <t>target_traj</t>
-  </si>
-  <si>
-    <t>trajectory (X,Y,Z) in time</t>
-  </si>
-  <si>
     <t>target_rt</t>
   </si>
   <si>
@@ -150,9 +143,6 @@
     <t>sub categorized target correctly: yes(1) / no(0)</t>
   </si>
   <si>
-    <t>prime_traj</t>
-  </si>
-  <si>
     <t>prime_rt</t>
   </si>
   <si>
@@ -160,9 +150,6 @@
   </si>
   <si>
     <t>correct on recognition task: yes(1) / no(0)</t>
-  </si>
-  <si>
-    <t>pas_traj</t>
   </si>
   <si>
     <t>pas</t>
@@ -279,12 +266,48 @@
   </si>
   <si>
     <t>subject number</t>
+  </si>
+  <si>
+    <t>pas_z</t>
+  </si>
+  <si>
+    <t>pas_x</t>
+  </si>
+  <si>
+    <t>pas_y</t>
+  </si>
+  <si>
+    <t>X trajectory in time</t>
+  </si>
+  <si>
+    <t>Y trajectory in time</t>
+  </si>
+  <si>
+    <t>Z trajectory in time</t>
+  </si>
+  <si>
+    <t>prime_x</t>
+  </si>
+  <si>
+    <t>prime_y</t>
+  </si>
+  <si>
+    <t>prime_z</t>
+  </si>
+  <si>
+    <t>target_x</t>
+  </si>
+  <si>
+    <t>target_y</t>
+  </si>
+  <si>
+    <t>target_z</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -599,19 +622,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AU2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AU3" sqref="AU3"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.25" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="46" max="46" width="20.5" customWidth="1"/>
+    <col min="52" max="52" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -631,37 +654,37 @@
         <v>19</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>1</v>
@@ -682,79 +705,97 @@
         <v>26</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AA1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AH1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AB1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AF1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AU1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AK1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AT1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>79</v>
+      <c r="AZ1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:47" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:53" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>29</v>
@@ -774,13 +815,13 @@
         <v>23</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>9</v>
@@ -801,92 +842,110 @@
         <v>27</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="S2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="X2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="W2" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>78</v>
-      </c>
       <c r="AA2" s="1" t="s">
-        <v>34</v>
+        <v>80</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>49</v>
+        <v>82</v>
       </c>
       <c r="AD2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AE2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AG2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AH2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AG2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AH2" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="AI2" s="1" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="AJ2" s="1" t="s">
-        <v>41</v>
+        <v>81</v>
       </c>
       <c r="AK2" s="1" t="s">
-        <v>13</v>
+        <v>82</v>
       </c>
       <c r="AL2" s="1" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="AM2" s="1" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="AN2" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="AO2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="AP2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AR2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AS2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AT2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AU2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AV2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AQ2" s="1"/>
-      <c r="AR2" s="1" t="s">
+      <c r="AW2" s="1"/>
+      <c r="AX2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AS2" s="1" t="s">
+      <c r="AY2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AT2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU2" s="1" t="s">
-        <v>80</v>
+      <c r="AZ2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="BA2" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Debug last 6 commits
</commit_message>
<xml_diff>
--- a/development/Code_Output_Explanation.xlsx
+++ b/development/Code_Output_Explanation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\khen_heller\subliminal_priming_w_motion_capture-main\development\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\My Drive\MudrikLab020818\Experiments_new\subliminal_priming_w_motion_capture\development\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="97">
   <si>
     <t>prime</t>
   </si>
@@ -196,18 +196,6 @@
 Screen(‘MakeTexture’)</t>
   </si>
   <si>
-    <t>time of each trajectory sample (sec)</t>
-  </si>
-  <si>
-    <t>pas_timecourse</t>
-  </si>
-  <si>
-    <t>prime_timecourse</t>
-  </si>
-  <si>
-    <t>target_timecourse</t>
-  </si>
-  <si>
     <t>fix_duration</t>
   </si>
   <si>
@@ -268,40 +256,76 @@
     <t>subject number</t>
   </si>
   <si>
-    <t>pas_z</t>
-  </si>
-  <si>
-    <t>pas_x</t>
-  </si>
-  <si>
-    <t>pas_y</t>
-  </si>
-  <si>
-    <t>X trajectory in time</t>
-  </si>
-  <si>
-    <t>Y trajectory in time</t>
-  </si>
-  <si>
-    <t>Z trajectory in time</t>
-  </si>
-  <si>
-    <t>prime_x</t>
-  </si>
-  <si>
-    <t>prime_y</t>
-  </si>
-  <si>
-    <t>prime_z</t>
-  </si>
-  <si>
-    <t>target_x</t>
-  </si>
-  <si>
-    <t>target_y</t>
-  </si>
-  <si>
-    <t>target_z</t>
+    <t>target_x_to</t>
+  </si>
+  <si>
+    <t>target_y_to</t>
+  </si>
+  <si>
+    <t>target_z_to</t>
+  </si>
+  <si>
+    <t>X trajectory to screen</t>
+  </si>
+  <si>
+    <t>Y trajectory to screen</t>
+  </si>
+  <si>
+    <t>Z trajectory to screen</t>
+  </si>
+  <si>
+    <t>target_timecourse_to</t>
+  </si>
+  <si>
+    <t>time of each trajectory sample (sec) when reaching to screen</t>
+  </si>
+  <si>
+    <t>target_x_from</t>
+  </si>
+  <si>
+    <t>target_y_from</t>
+  </si>
+  <si>
+    <t>target_z_from</t>
+  </si>
+  <si>
+    <t>target_timecourse_from</t>
+  </si>
+  <si>
+    <t>X trajectory from screen to start point</t>
+  </si>
+  <si>
+    <t>Y trajectory from screen to start point</t>
+  </si>
+  <si>
+    <t>Z trajectory from screen to start point</t>
+  </si>
+  <si>
+    <t>time of each trajectory sample (sec) when returning from screen</t>
+  </si>
+  <si>
+    <t>prime_x_to</t>
+  </si>
+  <si>
+    <t>prime_y_to</t>
+  </si>
+  <si>
+    <t>prime_z_to</t>
+  </si>
+  <si>
+    <t>prime_timecourse_to</t>
+  </si>
+  <si>
+    <t>prime_x_from</t>
+  </si>
+  <si>
+    <t>prime_y_from</t>
+  </si>
+  <si>
+    <t>prime_z_from</t>
+  </si>
+  <si>
+    <t>prime_timecourse_from</t>
   </si>
 </sst>
 </file>
@@ -623,18 +647,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA2"/>
+  <dimension ref="A1:BE2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W17" sqref="W17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.25" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="52" max="52" width="20.5" customWidth="1"/>
+    <col min="56" max="56" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:57" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -669,22 +693,22 @@
         <v>51</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>1</v>
@@ -705,97 +729,109 @@
         <v>26</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="AE1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AI1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="AM1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AU1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AP1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="BA1" s="1" t="s">
-        <v>75</v>
+      <c r="BE1" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:53" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:57" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>29</v>
@@ -842,110 +878,122 @@
         <v>27</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="S2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="X2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="W2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="AA2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AB2" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="AE2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AI2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AJ2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AK2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AH2" s="1" t="s">
+      <c r="AL2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AI2" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AJ2" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AK2" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AL2" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="AM2" s="1" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="AN2" s="1" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
       <c r="AO2" s="1" t="s">
-        <v>13</v>
+        <v>78</v>
       </c>
       <c r="AP2" s="1" t="s">
         <v>80</v>
       </c>
       <c r="AQ2" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="AR2" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="AS2" s="1" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="AT2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AU2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AV2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AW2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AX2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AU2" s="1" t="s">
+      <c r="AY2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AV2" s="1" t="s">
+      <c r="AZ2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AW2" s="1"/>
-      <c r="AX2" s="1" t="s">
+      <c r="BA2" s="1"/>
+      <c r="BB2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AY2" s="1" t="s">
+      <c r="BC2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AZ2" s="1" t="s">
+      <c r="BD2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="BA2" s="1" t="s">
-        <v>76</v>
+      <c r="BE2" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
trial, block_num --> iTrial, iBlock
</commit_message>
<xml_diff>
--- a/development/Code_Output_Explanation.xlsx
+++ b/development/Code_Output_Explanation.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\My Drive\MudrikLab020818\Experiments_new\subliminal_priming_w_motion_capture\development\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\university\mudrick_lab\subliminal_priming_w_motion_capture\development\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4FF026-B48F-4400-BEA0-8B5C74C15D55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,15 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -56,12 +48,6 @@
     <t>trial_end_time</t>
   </si>
   <si>
-    <t>trial</t>
-  </si>
-  <si>
-    <t>block_num</t>
-  </si>
-  <si>
     <t>Fixation duration</t>
   </si>
   <si>
@@ -326,12 +312,18 @@
   </si>
   <si>
     <t>prime_timecourse_from</t>
+  </si>
+  <si>
+    <t>iTrial</t>
+  </si>
+  <si>
+    <t>iBlock</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -646,11 +638,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BE2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W17" sqref="W17"/>
+    <sheetView tabSelected="1" topLeftCell="AY1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BC2" sqref="BC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.25" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -663,52 +655,52 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>1</v>
@@ -723,94 +715,94 @@
         <v>3</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="X1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="AA1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AB1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="AD1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AG1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AG1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="AI1" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="AJ1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AK1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AW1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AL1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AW1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="AY1" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="AZ1" s="1" t="s">
         <v>5</v>
@@ -819,181 +811,181 @@
         <v>6</v>
       </c>
       <c r="BB1" s="1" t="s">
-        <v>7</v>
+        <v>95</v>
       </c>
       <c r="BC1" s="1" t="s">
-        <v>8</v>
+        <v>96</v>
       </c>
       <c r="BD1" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="BE1" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:57" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="I2" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="AM2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AP2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AR2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AS2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AT2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AU2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AV2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AW2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AX2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AY2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AZ2" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AF2" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AG2" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AH2" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AI2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AJ2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AK2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AL2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AM2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="AN2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AO2" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AP2" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AQ2" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AR2" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AS2" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AT2" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AU2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AV2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AW2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AX2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AY2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AZ2" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="BA2" s="1"/>
       <c r="BB2" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="BC2" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="BD2" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="BE2" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve trial shuffle | Added SubNum to traj output file
no consequent distractors.
</commit_message>
<xml_diff>
--- a/development/Code_Output_Explanation.xlsx
+++ b/development/Code_Output_Explanation.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\university\mudrick_lab\subliminal_priming_w_motion_capture\development\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\khen_heller\subliminal_priming_w_motion_capture\development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4FF026-B48F-4400-BEA0-8B5C74C15D55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -323,7 +322,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -638,16 +637,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BE2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AY1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BC2" sqref="BC2"/>
+      <selection activeCell="BD7" sqref="BD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.25" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="56" max="56" width="20.5" customWidth="1"/>
+    <col min="57" max="57" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:57" ht="28.5" x14ac:dyDescent="0.2">
@@ -811,16 +810,16 @@
         <v>6</v>
       </c>
       <c r="BB1" s="1" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="BC1" s="1" t="s">
         <v>96</v>
       </c>
       <c r="BD1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="BE1" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="BE1" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:57" ht="71.25" x14ac:dyDescent="0.2">
@@ -976,16 +975,16 @@
       </c>
       <c r="BA2" s="1"/>
       <c r="BB2" s="1" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="BC2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="BD2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="BE2" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="BE2" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated docs | added global in getTraj.m
</commit_message>
<xml_diff>
--- a/development/Code_Output_Explanation.xlsx
+++ b/development/Code_Output_Explanation.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\khen_heller\subliminal_priming_w_motion_capture\development\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\university\mudrick_lab\subliminal_priming_w_motion_capture\development\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB70C01D-69CA-471A-9AA4-FFF33F44556D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -158,9 +159,6 @@
     <t>What the subject chose: left(1) / right(0)</t>
   </si>
   <si>
-    <t>same_w</t>
-  </si>
-  <si>
     <t>cat_block</t>
   </si>
   <si>
@@ -317,12 +315,15 @@
   </si>
   <si>
     <t>iBlock</t>
+  </si>
+  <si>
+    <t>same</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -637,11 +638,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BE2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AY1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BD7" sqref="BD7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.25" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -669,37 +670,37 @@
         <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="L1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>1</v>
@@ -720,37 +721,37 @@
         <v>24</v>
       </c>
       <c r="X1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="AA1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AC1" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="AD1" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AE1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AF1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="AI1" s="1" t="s">
         <v>42</v>
@@ -765,28 +766,28 @@
         <v>31</v>
       </c>
       <c r="AM1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AN1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="AU1" s="1" t="s">
         <v>39</v>
@@ -810,16 +811,16 @@
         <v>6</v>
       </c>
       <c r="BB1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BC1" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="BD1" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="BE1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:57" ht="71.25" x14ac:dyDescent="0.2">
@@ -842,13 +843,13 @@
         <v>21</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>7</v>
@@ -869,55 +870,55 @@
         <v>25</v>
       </c>
       <c r="R2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="S2" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="T2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="U2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="Z2" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="AA2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AC2" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="AD2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AE2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AG2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AH2" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="AH2" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="AI2" s="1" t="s">
         <v>43</v>
@@ -932,28 +933,28 @@
         <v>11</v>
       </c>
       <c r="AM2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AN2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="AN2" s="1" t="s">
+      <c r="AO2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AO2" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="AP2" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AQ2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AR2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="AR2" s="1" t="s">
+      <c r="AS2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AS2" s="1" t="s">
+      <c r="AT2" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="AT2" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="AU2" s="1" t="s">
         <v>40</v>
@@ -975,7 +976,7 @@
       </c>
       <c r="BA2" s="1"/>
       <c r="BB2" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="BC2" s="1" t="s">
         <v>14</v>
@@ -984,7 +985,7 @@
         <v>13</v>
       </c>
       <c r="BE2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
turn tests to standalone | Add practice field in output file
</commit_message>
<xml_diff>
--- a/development/Code_Output_Explanation.xlsx
+++ b/development/Code_Output_Explanation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\university\mudrick_lab\subliminal_priming_w_motion_capture\development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB70C01D-69CA-471A-9AA4-FFF33F44556D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC8456C-9145-444D-A985-FD33D247A276}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="99">
   <si>
     <t>prime</t>
   </si>
@@ -157,13 +157,6 @@
   </si>
   <si>
     <t>What the subject chose: left(1) / right(0)</t>
-  </si>
-  <si>
-    <t>cat_block</t>
-  </si>
-  <si>
-    <t>block type: 
-target categorization(1) / prime recognition(0)</t>
   </si>
   <si>
     <t>mask1</t>
@@ -318,6 +311,18 @@
   </si>
   <si>
     <t>same</t>
+  </si>
+  <si>
+    <t>list_id</t>
+  </si>
+  <si>
+    <t>Name of trials list used for this subject</t>
+  </si>
+  <si>
+    <t>practice</t>
+  </si>
+  <si>
+    <t>Indicates this is a practice trial.</t>
   </si>
 </sst>
 </file>
@@ -639,354 +644,357 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BE2"/>
+  <dimension ref="A1:BF2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.25" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="57" max="57" width="20.5" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:57" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:58" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="BD1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:58" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="P1" s="1" t="s">
+      <c r="O2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="W2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AA1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AA2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AG2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="AD1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AK2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AI1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AY1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="BB1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="BC1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="BD1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="BE1" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:57" ht="71.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AL2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AP2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AR2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AS2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AT2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="AB2" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AU2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="AD2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AV2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AW2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AX2" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AY2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="AG2" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AH2" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AI2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AJ2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AK2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AL2" s="1" t="s">
+      <c r="AZ2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="BA2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="BB2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AM2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AN2" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AO2" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="AP2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="AQ2" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AR2" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AS2" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AT2" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AU2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AV2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AW2" s="1" t="s">
+      <c r="BC2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="BD2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AX2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AY2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AZ2" s="1" t="s">
+      <c r="BE2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="BA2" s="1"/>
-      <c r="BB2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BC2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="BD2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="BE2" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="BF2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>